<commit_message>
Add file of county extreme rainfall years
</commit_message>
<xml_diff>
--- a/Locations/County-Extreme-Rainfall-Years.xlsx
+++ b/Locations/County-Extreme-Rainfall-Years.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\DQ_Checks\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\Locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4670BC-77AA-4FC3-A8F2-9D2379B738D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A484DBA-4E5C-450B-9A45-27E2028C58F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="By Year" sheetId="1" r:id="rId1"/>
-    <sheet name="By County" sheetId="2" r:id="rId2"/>
+    <sheet name="By County" sheetId="2" r:id="rId1"/>
+    <sheet name="By Year" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'By County'!$A$1:$J$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'By County'!$A$1:$J$91</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -1530,1547 +1530,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H141"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B92" sqref="B92"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="35.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="35.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1821</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1821</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1822</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1823</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1823</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1824</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1825</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>1826</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="6">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>1827</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>1828</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1828</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>1829</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>1830</v>
-      </c>
-      <c r="E11" s="6">
-        <v>1830</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>1831</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1831</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>1832</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1832</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>1833</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>1834</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1834</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>1835</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1835</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>1836</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1836</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>1837</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>1838</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1838</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>1839</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1839</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>1840</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1840</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>1841</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1841</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>1842</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1842</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>1843</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1843</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>1844</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="6">
-        <v>1844</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>1845</v>
-      </c>
-      <c r="E26" s="6">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>1846</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1846</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>1847</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="6">
-        <v>1847</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>1848</v>
-      </c>
-      <c r="E29" s="6">
-        <v>1848</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>1849</v>
-      </c>
-      <c r="E30" s="6">
-        <v>1849</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>1850</v>
-      </c>
-      <c r="E31" s="6">
-        <v>1850</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>1851</v>
-      </c>
-      <c r="E32" s="6">
-        <v>1851</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>1852</v>
-      </c>
-      <c r="E33" s="6">
-        <v>1852</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>1853</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="6">
-        <v>1853</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>1854</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="6">
-        <v>1854</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="6">
-        <v>1855</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>1856</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="6">
-        <v>1856</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>1857</v>
-      </c>
-      <c r="E38" s="6">
-        <v>1857</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>1858</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" s="6">
-        <v>1858</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>1859</v>
-      </c>
-      <c r="E40" s="6">
-        <v>1859</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>1860</v>
-      </c>
-      <c r="E41" s="6">
-        <v>1860</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
-        <v>1861</v>
-      </c>
-      <c r="E42" s="6">
-        <v>1861</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>1862</v>
-      </c>
-      <c r="E43" s="6">
-        <v>1862</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>1863</v>
-      </c>
-      <c r="E44" s="6">
-        <v>1863</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>1864</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="6">
-        <v>1864</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
-        <v>1865</v>
-      </c>
-      <c r="E46" s="6">
-        <v>1865</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>1866</v>
-      </c>
-      <c r="E47" s="6">
-        <v>1866</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>1867</v>
-      </c>
-      <c r="E48" s="6">
-        <v>1867</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
-        <v>1868</v>
-      </c>
-      <c r="E49" s="6">
-        <v>1868</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>1869</v>
-      </c>
-      <c r="E50" s="6">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>1870</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" s="6">
-        <v>1870</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>1871</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="6">
-        <v>1871</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>1872</v>
-      </c>
-      <c r="E53" s="6">
-        <v>1872</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>1873</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E54" s="6">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
-        <v>1874</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="6">
-        <v>1874</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
-        <v>1875</v>
-      </c>
-      <c r="E56" s="6">
-        <v>1875</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
-        <v>1876</v>
-      </c>
-      <c r="E57" s="6">
-        <v>1876</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
-        <v>1877</v>
-      </c>
-      <c r="E58" s="6">
-        <v>1877</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
-        <v>1878</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E59" s="6">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
-        <v>1879</v>
-      </c>
-      <c r="E60" s="6">
-        <v>1879</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
-        <v>1880</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E61" s="6">
-        <v>1880</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
-        <v>1881</v>
-      </c>
-      <c r="E62" s="6">
-        <v>1881</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
-        <v>1882</v>
-      </c>
-      <c r="E63" s="6">
-        <v>1882</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
-        <v>1883</v>
-      </c>
-      <c r="E64" s="6">
-        <v>1883</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
-        <v>1884</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E65" s="6">
-        <v>1884</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
-        <v>1885</v>
-      </c>
-      <c r="E66" s="6">
-        <v>1885</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
-        <v>1886</v>
-      </c>
-      <c r="E67" s="6">
-        <v>1886</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
-        <v>1887</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E68" s="6">
-        <v>1887</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
-        <v>1888</v>
-      </c>
-      <c r="E69" s="6">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
-        <v>1889</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E70" s="6">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
-        <v>1890</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E71" s="6">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
-        <v>1891</v>
-      </c>
-      <c r="E72" s="6">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
-        <v>1892</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73" s="6">
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
-        <v>1893</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E74" s="6">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
-        <v>1894</v>
-      </c>
-      <c r="E75" s="6">
-        <v>1894</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
-        <v>1895</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E76" s="6">
-        <v>1895</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
-        <v>1896</v>
-      </c>
-      <c r="E77" s="6">
-        <v>1896</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
-        <v>1897</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E78" s="6">
-        <v>1897</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
-        <v>1898</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E79" s="6">
-        <v>1898</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="4">
-        <v>1899</v>
-      </c>
-      <c r="E80" s="6">
-        <v>1899</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
-        <v>1900</v>
-      </c>
-      <c r="E81" s="6">
-        <v>1900</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
-        <v>1901</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E82" s="6">
-        <v>1901</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
-        <v>1902</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E83" s="6">
-        <v>1902</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
-        <v>1903</v>
-      </c>
-      <c r="E84" s="6">
-        <v>1903</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
-        <v>1904</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E85" s="6">
-        <v>1904</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
-        <v>1905</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E86" s="6">
-        <v>1905</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
-        <v>1906</v>
-      </c>
-      <c r="E87" s="6">
-        <v>1906</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
-        <v>1907</v>
-      </c>
-      <c r="E88" s="6">
-        <v>1907</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
-        <v>1908</v>
-      </c>
-      <c r="E89" s="6">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
-        <v>1909</v>
-      </c>
-      <c r="E90" s="6">
-        <v>1909</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
-        <v>1910</v>
-      </c>
-      <c r="E91" s="6">
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
-        <v>1911</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E92" s="6">
-        <v>1911</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
-        <v>1912</v>
-      </c>
-      <c r="E93" s="6">
-        <v>1912</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
-        <v>1913</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E94" s="6">
-        <v>1913</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
-        <v>1914</v>
-      </c>
-      <c r="E95" s="6">
-        <v>1914</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
-        <v>1915</v>
-      </c>
-      <c r="E96" s="6">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
-        <v>1916</v>
-      </c>
-      <c r="E97" s="6">
-        <v>1916</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
-        <v>1917</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E98" s="6">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
-        <v>1918</v>
-      </c>
-      <c r="E99" s="6">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
-        <v>1919</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E100" s="6">
-        <v>1919</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
-        <v>1920</v>
-      </c>
-      <c r="E101" s="6">
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
-        <v>1921</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E102" s="6">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
-        <v>1922</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E103" s="6">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
-        <v>1923</v>
-      </c>
-      <c r="E104" s="6">
-        <v>1923</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="4">
-        <v>1924</v>
-      </c>
-      <c r="E105" s="6">
-        <v>1924</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H105" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
-        <v>1925</v>
-      </c>
-      <c r="E106" s="6">
-        <v>1925</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
-        <v>1926</v>
-      </c>
-      <c r="E107" s="6">
-        <v>1926</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
-        <v>1927</v>
-      </c>
-      <c r="E108" s="6">
-        <v>1927</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A109" s="4">
-        <v>1928</v>
-      </c>
-      <c r="E109" s="6">
-        <v>1928</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H109" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="4">
-        <v>1929</v>
-      </c>
-      <c r="E110" s="6">
-        <v>1929</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
-        <v>1930</v>
-      </c>
-      <c r="E111" s="6">
-        <v>1930</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H111" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="4">
-        <v>1931</v>
-      </c>
-      <c r="E112" s="6">
-        <v>1931</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="4">
-        <v>1932</v>
-      </c>
-      <c r="E113" s="6">
-        <v>1932</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A114" s="4">
-        <v>1933</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E114" s="6">
-        <v>1933</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="4">
-        <v>1934</v>
-      </c>
-      <c r="E115" s="6">
-        <v>1934</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
-        <v>1935</v>
-      </c>
-      <c r="E116" s="6">
-        <v>1935</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
-        <v>1936</v>
-      </c>
-      <c r="E117" s="6">
-        <v>1936</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="4">
-        <v>1937</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E118" s="6">
-        <v>1937</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
-        <v>1938</v>
-      </c>
-      <c r="E119" s="6">
-        <v>1938</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="4">
-        <v>1939</v>
-      </c>
-      <c r="E120" s="6">
-        <v>1939</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="4">
-        <v>1940</v>
-      </c>
-      <c r="E121" s="6">
-        <v>1940</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="4">
-        <v>1941</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E122" s="6">
-        <v>1941</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="4">
-        <v>1942</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E123" s="6">
-        <v>1942</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="4">
-        <v>1943</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E124" s="6">
-        <v>1943</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="4">
-        <v>1944</v>
-      </c>
-      <c r="E125" s="6">
-        <v>1944</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="4">
-        <v>1945</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E126" s="6">
-        <v>1945</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="4">
-        <v>1946</v>
-      </c>
-      <c r="E127" s="6">
-        <v>1946</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="4">
-        <v>1947</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E128" s="6">
-        <v>1947</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A129" s="4">
-        <v>1948</v>
-      </c>
-      <c r="E129" s="6">
-        <v>1948</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
-        <v>1949</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E130" s="6">
-        <v>1949</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="4">
-        <v>1950</v>
-      </c>
-      <c r="E131" s="6">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="4">
-        <v>1951</v>
-      </c>
-      <c r="E132" s="6">
-        <v>1951</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="4">
-        <v>1952</v>
-      </c>
-      <c r="E133" s="6">
-        <v>1952</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
-        <v>1953</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E134" s="6">
-        <v>1953</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A135" s="4">
-        <v>1954</v>
-      </c>
-      <c r="E135" s="6">
-        <v>1954</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H135" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
-        <v>1955</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E136" s="6">
-        <v>1955</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="4">
-        <v>1956</v>
-      </c>
-      <c r="E137" s="6">
-        <v>1956</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
-        <v>1957</v>
-      </c>
-      <c r="E138" s="6">
-        <v>1957</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="4">
-        <v>1958</v>
-      </c>
-      <c r="E139" s="6">
-        <v>1958</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A140" s="4">
-        <v>1959</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E140" s="6">
-        <v>1959</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A141" s="4">
-        <v>1960</v>
-      </c>
-      <c r="E141" s="6">
-        <v>1960</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G141" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H141" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A66364B-DE42-45C8-AFCC-528046C40C07}">
   <dimension ref="A1:J91"/>
   <sheetViews>
@@ -5606,4 +4065,1545 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H141"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="35.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="35.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1821</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1822</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1823</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1824</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1825</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1826</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1827</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1828</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1829</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1830</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1830</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1831</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1832</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1833</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1834</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1835</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1836</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1836</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>1837</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>1838</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>1839</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1840</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1841</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1841</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1842</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>1843</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1844</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1845</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1846</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1847</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1848</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1848</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1849</v>
+      </c>
+      <c r="E30" s="6">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1850</v>
+      </c>
+      <c r="E31" s="6">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>1851</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1852</v>
+      </c>
+      <c r="E33" s="6">
+        <v>1852</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1853</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="6">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1854</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>1856</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="6">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>1857</v>
+      </c>
+      <c r="E38" s="6">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>1858</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="6">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>1859</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1859</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>1860</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>1861</v>
+      </c>
+      <c r="E42" s="6">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>1862</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>1863</v>
+      </c>
+      <c r="E44" s="6">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>1864</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="6">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1865</v>
+      </c>
+      <c r="E46" s="6">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>1866</v>
+      </c>
+      <c r="E47" s="6">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>1867</v>
+      </c>
+      <c r="E48" s="6">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>1868</v>
+      </c>
+      <c r="E49" s="6">
+        <v>1868</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>1869</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>1870</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="6">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>1871</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="6">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>1872</v>
+      </c>
+      <c r="E53" s="6">
+        <v>1872</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>1873</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="6">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>1874</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="6">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>1875</v>
+      </c>
+      <c r="E56" s="6">
+        <v>1875</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>1876</v>
+      </c>
+      <c r="E57" s="6">
+        <v>1876</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>1877</v>
+      </c>
+      <c r="E58" s="6">
+        <v>1877</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>1878</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E59" s="6">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>1879</v>
+      </c>
+      <c r="E60" s="6">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>1880</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" s="6">
+        <v>1880</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>1881</v>
+      </c>
+      <c r="E62" s="6">
+        <v>1881</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>1882</v>
+      </c>
+      <c r="E63" s="6">
+        <v>1882</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>1883</v>
+      </c>
+      <c r="E64" s="6">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>1884</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" s="6">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>1885</v>
+      </c>
+      <c r="E66" s="6">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>1886</v>
+      </c>
+      <c r="E67" s="6">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>1887</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="6">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>1888</v>
+      </c>
+      <c r="E69" s="6">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>1889</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" s="6">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>1890</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E71" s="6">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>1891</v>
+      </c>
+      <c r="E72" s="6">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>1892</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" s="6">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1893</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E74" s="6">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>1894</v>
+      </c>
+      <c r="E75" s="6">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>1895</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E76" s="6">
+        <v>1895</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>1896</v>
+      </c>
+      <c r="E77" s="6">
+        <v>1896</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>1897</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E78" s="6">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>1898</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E79" s="6">
+        <v>1898</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>1899</v>
+      </c>
+      <c r="E80" s="6">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>1900</v>
+      </c>
+      <c r="E81" s="6">
+        <v>1900</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>1901</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E82" s="6">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>1902</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E83" s="6">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>1903</v>
+      </c>
+      <c r="E84" s="6">
+        <v>1903</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>1904</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E85" s="6">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>1905</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E86" s="6">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>1906</v>
+      </c>
+      <c r="E87" s="6">
+        <v>1906</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>1907</v>
+      </c>
+      <c r="E88" s="6">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>1908</v>
+      </c>
+      <c r="E89" s="6">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>1909</v>
+      </c>
+      <c r="E90" s="6">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>1910</v>
+      </c>
+      <c r="E91" s="6">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>1911</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E92" s="6">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>1912</v>
+      </c>
+      <c r="E93" s="6">
+        <v>1912</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>1913</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E94" s="6">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>1914</v>
+      </c>
+      <c r="E95" s="6">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>1915</v>
+      </c>
+      <c r="E96" s="6">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>1916</v>
+      </c>
+      <c r="E97" s="6">
+        <v>1916</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>1917</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E98" s="6">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>1918</v>
+      </c>
+      <c r="E99" s="6">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>1919</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E100" s="6">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>1920</v>
+      </c>
+      <c r="E101" s="6">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
+        <v>1921</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E102" s="6">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>1922</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E103" s="6">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <v>1923</v>
+      </c>
+      <c r="E104" s="6">
+        <v>1923</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <v>1924</v>
+      </c>
+      <c r="E105" s="6">
+        <v>1924</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>1925</v>
+      </c>
+      <c r="E106" s="6">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <v>1926</v>
+      </c>
+      <c r="E107" s="6">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>1927</v>
+      </c>
+      <c r="E108" s="6">
+        <v>1927</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>1928</v>
+      </c>
+      <c r="E109" s="6">
+        <v>1928</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <v>1929</v>
+      </c>
+      <c r="E110" s="6">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <v>1930</v>
+      </c>
+      <c r="E111" s="6">
+        <v>1930</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <v>1931</v>
+      </c>
+      <c r="E112" s="6">
+        <v>1931</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
+        <v>1932</v>
+      </c>
+      <c r="E113" s="6">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A114" s="4">
+        <v>1933</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E114" s="6">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <v>1934</v>
+      </c>
+      <c r="E115" s="6">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <v>1935</v>
+      </c>
+      <c r="E116" s="6">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="4">
+        <v>1936</v>
+      </c>
+      <c r="E117" s="6">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <v>1937</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E118" s="6">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
+        <v>1938</v>
+      </c>
+      <c r="E119" s="6">
+        <v>1938</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <v>1939</v>
+      </c>
+      <c r="E120" s="6">
+        <v>1939</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <v>1940</v>
+      </c>
+      <c r="E121" s="6">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="4">
+        <v>1941</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E122" s="6">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="4">
+        <v>1942</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E123" s="6">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="4">
+        <v>1943</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E124" s="6">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="4">
+        <v>1944</v>
+      </c>
+      <c r="E125" s="6">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="4">
+        <v>1945</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E126" s="6">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
+        <v>1946</v>
+      </c>
+      <c r="E127" s="6">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="4">
+        <v>1947</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E128" s="6">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A129" s="4">
+        <v>1948</v>
+      </c>
+      <c r="E129" s="6">
+        <v>1948</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="4">
+        <v>1949</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E130" s="6">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="4">
+        <v>1950</v>
+      </c>
+      <c r="E131" s="6">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="4">
+        <v>1951</v>
+      </c>
+      <c r="E132" s="6">
+        <v>1951</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="4">
+        <v>1952</v>
+      </c>
+      <c r="E133" s="6">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="4">
+        <v>1953</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E134" s="6">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A135" s="4">
+        <v>1954</v>
+      </c>
+      <c r="E135" s="6">
+        <v>1954</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A136" s="4">
+        <v>1955</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E136" s="6">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="4">
+        <v>1956</v>
+      </c>
+      <c r="E137" s="6">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="4">
+        <v>1957</v>
+      </c>
+      <c r="E138" s="6">
+        <v>1957</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="4">
+        <v>1958</v>
+      </c>
+      <c r="E139" s="6">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="4">
+        <v>1959</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E140" s="6">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A141" s="4">
+        <v>1960</v>
+      </c>
+      <c r="E141" s="6">
+        <v>1960</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>